<commit_message>
first sb and fa phx las routes generated/formatted
</commit_message>
<xml_diff>
--- a/PHX-LV/flightData/path/PHX_LAS_022124_1.xlsx
+++ b/PHX-LV/flightData/path/PHX_LAS_022124_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashle\Documents\GitHub\Honeywell-Project\PHX-LV\flightData\path\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDB031A-95DC-45F1-92E9-AA7903FDCF35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B07E40-3435-4251-A666-E39C67DEB03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{909676FB-2349-4122-885D-57CD1045AA36}"/>
   </bookViews>
@@ -1236,7 +1236,7 @@
   <dimension ref="A1:L102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>